<commit_message>
started revamp of calculate_positions
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
   <si>
     <t>Today's date:</t>
   </si>
@@ -240,6 +240,21 @@
   </si>
   <si>
     <t>ON HOLD</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>o1</t>
+  </si>
+  <si>
+    <t>o2</t>
   </si>
 </sst>
 </file>
@@ -249,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-dd\-yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -264,9 +279,13 @@
     <font>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -309,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -328,9 +347,7 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -349,6 +366,20 @@
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,7 +485,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O17" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O22" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="14">
     <tableColumn name="Project _x000a_ID" id="1"/>
     <tableColumn name="Project Name" id="2"/>
@@ -706,7 +737,7 @@
       </c>
       <c r="C1" s="2">
         <f>TODAY()</f>
-        <v>45499</v>
+        <v>45500</v>
       </c>
     </row>
     <row r="2" ht="58.5" customHeight="1">
@@ -807,7 +838,7 @@
       </c>
       <c r="O3" s="13">
         <f t="shared" ref="O3:O17" si="2">IFERROR(IF($K3=1,0,IF(($C$1-$K3)/($M3-$K3)&lt;-0.005,100%,IF(($C$1-$K3)/($M3-$K3)&gt;100%,100%,($C$1-$K3)/($L3-$K3)))),0)</f>
-        <v>0.6424968474</v>
+        <v>0.6443883985</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
@@ -897,7 +928,7 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" si="2"/>
-        <v>0.6524137931</v>
+        <v>0.6565517241</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
@@ -942,7 +973,7 @@
       </c>
       <c r="O6" s="13">
         <f t="shared" si="2"/>
-        <v>0.4740425532</v>
+        <v>0.4765957447</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
@@ -987,7 +1018,7 @@
       </c>
       <c r="O7" s="13">
         <f t="shared" si="2"/>
-        <v>0.9026876738</v>
+        <v>0.9054680259</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
@@ -1077,7 +1108,7 @@
       </c>
       <c r="O9" s="13">
         <f t="shared" si="2"/>
-        <v>0.8477537438</v>
+        <v>0.850249584</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
@@ -1167,7 +1198,7 @@
       </c>
       <c r="O11" s="13">
         <f t="shared" si="2"/>
-        <v>0.9723502304</v>
+        <v>0.9792626728</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="1">
@@ -1212,7 +1243,7 @@
       </c>
       <c r="O12" s="13">
         <f t="shared" si="2"/>
-        <v>0.2773279352</v>
+        <v>0.2834008097</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="1">
@@ -1257,7 +1288,7 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" si="2"/>
-        <v>0.3803278689</v>
+        <v>0.3901639344</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="1">
@@ -1302,7 +1333,7 @@
       </c>
       <c r="O14" s="13">
         <f t="shared" si="2"/>
-        <v>0.9952992792</v>
+        <v>0.9962394234</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
@@ -1347,7 +1378,7 @@
       </c>
       <c r="O15" s="13">
         <f t="shared" si="2"/>
-        <v>0.7700084246</v>
+        <v>0.7725358045</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -1392,7 +1423,7 @@
       </c>
       <c r="O16" s="13">
         <f t="shared" si="2"/>
-        <v>0.7700084246</v>
+        <v>0.7725358045</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1437,14 +1468,129 @@
       </c>
       <c r="O17" s="13">
         <f t="shared" si="2"/>
-        <v>0.7700084246</v>
+        <v>0.7725358045</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="B18" s="16"/>
+      <c r="C18" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="B21" s="16"/>
+      <c r="C21" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="21">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="B22" s="16"/>
+      <c r="C22" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="21">
+        <v>0.77</v>
+      </c>
+    </row>
     <row r="23" ht="14.25" customHeight="1"/>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
@@ -1643,786 +1789,786 @@
     <row r="218" ht="14.25" customHeight="1"/>
     <row r="219" ht="14.25" customHeight="1"/>
     <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G3:G17">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
started angle bound alterations
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
   <si>
     <t>Today's date:</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>o2</t>
+  </si>
+  <si>
+    <t>o3</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -370,6 +373,8 @@
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -488,7 +493,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O22" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O23" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="14">
     <tableColumn name="Project _x000a_ID" id="1"/>
     <tableColumn name="Project Name" id="2"/>
@@ -740,7 +745,7 @@
       </c>
       <c r="C1" s="2">
         <f>TODAY()</f>
-        <v>45500</v>
+        <v>45501</v>
       </c>
     </row>
     <row r="2" ht="58.5" customHeight="1">
@@ -841,7 +846,7 @@
       </c>
       <c r="O3" s="13">
         <f t="shared" ref="O3:O17" si="2">IFERROR(IF($K3=1,0,IF(($C$1-$K3)/($M3-$K3)&lt;-0.005,100%,IF(($C$1-$K3)/($M3-$K3)&gt;100%,100%,($C$1-$K3)/($L3-$K3)))),0)</f>
-        <v>0.6443883985</v>
+        <v>0.6462799496</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
@@ -931,7 +936,7 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" si="2"/>
-        <v>0.6565517241</v>
+        <v>0.6606896552</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
@@ -976,7 +981,7 @@
       </c>
       <c r="O6" s="13">
         <f t="shared" si="2"/>
-        <v>0.4765957447</v>
+        <v>0.4791489362</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
@@ -1021,7 +1026,7 @@
       </c>
       <c r="O7" s="13">
         <f t="shared" si="2"/>
-        <v>0.9054680259</v>
+        <v>0.9082483781</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
@@ -1111,7 +1116,7 @@
       </c>
       <c r="O9" s="13">
         <f t="shared" si="2"/>
-        <v>0.850249584</v>
+        <v>0.8527454243</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
@@ -1201,7 +1206,7 @@
       </c>
       <c r="O11" s="13">
         <f t="shared" si="2"/>
-        <v>0.9792626728</v>
+        <v>0.9861751152</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="1">
@@ -1246,7 +1251,7 @@
       </c>
       <c r="O12" s="13">
         <f t="shared" si="2"/>
-        <v>0.2834008097</v>
+        <v>0.2894736842</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="1">
@@ -1291,7 +1296,7 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" si="2"/>
-        <v>0.3901639344</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="1">
@@ -1336,7 +1341,7 @@
       </c>
       <c r="O14" s="13">
         <f t="shared" si="2"/>
-        <v>0.9962394234</v>
+        <v>0.9971795675</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
@@ -1381,7 +1386,7 @@
       </c>
       <c r="O15" s="13">
         <f t="shared" si="2"/>
-        <v>0.7725358045</v>
+        <v>0.7750631845</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -1426,7 +1431,7 @@
       </c>
       <c r="O16" s="13">
         <f t="shared" si="2"/>
-        <v>0.7725358045</v>
+        <v>0.7750631845</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1471,130 +1476,153 @@
       </c>
       <c r="O17" s="13">
         <f t="shared" si="2"/>
-        <v>0.7725358045</v>
+        <v>0.7750631845</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="16"/>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="17" t="s">
+      <c r="H18" s="16"/>
+      <c r="I18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="21">
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="17">
         <v>1.0</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="17" t="s">
+      <c r="H19" s="16"/>
+      <c r="I19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="21">
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="17">
         <v>1.0</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="17" t="s">
+      <c r="H20" s="16"/>
+      <c r="I20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="21">
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="17">
         <v>1.0</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="17" t="s">
+      <c r="H21" s="16"/>
+      <c r="I21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="21">
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="17">
         <v>0.77</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="B22" s="16"/>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17" t="s">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="17" t="s">
+      <c r="H22" s="16"/>
+      <c r="I22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="21">
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="17">
         <v>0.77</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="20"/>
+      <c r="I23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="23">
+        <v>0.0</v>
+      </c>
+    </row>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
     <row r="26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add more data points
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
   <si>
     <t>Today's date:</t>
   </si>
@@ -260,7 +260,19 @@
     <t>o2</t>
   </si>
   <si>
-    <t>o3</t>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
   </si>
 </sst>
 </file>
@@ -296,7 +308,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +333,12 @@
         <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1E4F5"/>
+        <bgColor rgb="FFC1E4F5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -334,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -388,6 +406,22 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,7 +527,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O23" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O27" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="14">
     <tableColumn name="Project _x000a_ID" id="1"/>
     <tableColumn name="Project Name" id="2"/>
@@ -745,7 +779,7 @@
       </c>
       <c r="C1" s="2">
         <f>TODAY()</f>
-        <v>45501</v>
+        <v>45502</v>
       </c>
     </row>
     <row r="2" ht="58.5" customHeight="1">
@@ -846,7 +880,7 @@
       </c>
       <c r="O3" s="13">
         <f t="shared" ref="O3:O17" si="2">IFERROR(IF($K3=1,0,IF(($C$1-$K3)/($M3-$K3)&lt;-0.005,100%,IF(($C$1-$K3)/($M3-$K3)&gt;100%,100%,($C$1-$K3)/($L3-$K3)))),0)</f>
-        <v>0.6462799496</v>
+        <v>0.6481715006</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
@@ -936,7 +970,7 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" si="2"/>
-        <v>0.6606896552</v>
+        <v>0.6648275862</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
@@ -981,7 +1015,7 @@
       </c>
       <c r="O6" s="13">
         <f t="shared" si="2"/>
-        <v>0.4791489362</v>
+        <v>0.4817021277</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
@@ -1026,7 +1060,7 @@
       </c>
       <c r="O7" s="13">
         <f t="shared" si="2"/>
-        <v>0.9082483781</v>
+        <v>0.9110287303</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
@@ -1116,7 +1150,7 @@
       </c>
       <c r="O9" s="13">
         <f t="shared" si="2"/>
-        <v>0.8527454243</v>
+        <v>0.8552412646</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
@@ -1206,7 +1240,7 @@
       </c>
       <c r="O11" s="13">
         <f t="shared" si="2"/>
-        <v>0.9861751152</v>
+        <v>0.9930875576</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="1">
@@ -1251,7 +1285,7 @@
       </c>
       <c r="O12" s="13">
         <f t="shared" si="2"/>
-        <v>0.2894736842</v>
+        <v>0.2955465587</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="1">
@@ -1296,7 +1330,7 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" si="2"/>
-        <v>0.4</v>
+        <v>0.4098360656</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="1">
@@ -1341,7 +1375,7 @@
       </c>
       <c r="O14" s="13">
         <f t="shared" si="2"/>
-        <v>0.9971795675</v>
+        <v>0.9981197117</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
@@ -1386,7 +1420,7 @@
       </c>
       <c r="O15" s="13">
         <f t="shared" si="2"/>
-        <v>0.7750631845</v>
+        <v>0.7775905644</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -1431,7 +1465,7 @@
       </c>
       <c r="O16" s="13">
         <f t="shared" si="2"/>
-        <v>0.7750631845</v>
+        <v>0.7775905644</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1476,7 +1510,7 @@
       </c>
       <c r="O17" s="13">
         <f t="shared" si="2"/>
-        <v>0.7750631845</v>
+        <v>0.7775905644</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
@@ -1608,7 +1642,7 @@
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="19" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="19" t="s">
@@ -1620,13 +1654,107 @@
       <c r="M23" s="22"/>
       <c r="N23" s="18"/>
       <c r="O23" s="23">
-        <v>0.0</v>
+        <v>0.77</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="20"/>
+      <c r="I24" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="23">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="B25" s="24"/>
+      <c r="C25" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="I25" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="28">
+        <v>0.77</v>
+      </c>
+      <c r="P25" s="29"/>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="B26" s="24"/>
+      <c r="C26" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="24"/>
+      <c r="I26" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="28">
+        <v>0.77</v>
+      </c>
+      <c r="P26" s="29"/>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="B27" s="24"/>
+      <c r="C27" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="24"/>
+      <c r="I27" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="28">
+        <v>0.77</v>
+      </c>
+    </row>
     <row r="28" ht="14.25" customHeight="1"/>
     <row r="29" ht="14.25" customHeight="1"/>
     <row r="30" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add test data points
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
   <si>
     <t>Today's date:</t>
   </si>
@@ -273,6 +273,42 @@
   </si>
   <si>
     <t>a5</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>InfoSec Protection Services</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>IT Risk Management</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>Security Design Services</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>Compliance &amp; Assurance</t>
   </si>
 </sst>
 </file>
@@ -352,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -393,25 +429,8 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -422,6 +441,16 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,7 +556,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O27" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O35" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="14">
     <tableColumn name="Project _x000a_ID" id="1"/>
     <tableColumn name="Project Name" id="2"/>
@@ -779,7 +808,7 @@
       </c>
       <c r="C1" s="2">
         <f>TODAY()</f>
-        <v>45502</v>
+        <v>45503</v>
       </c>
     </row>
     <row r="2" ht="58.5" customHeight="1">
@@ -880,7 +909,7 @@
       </c>
       <c r="O3" s="13">
         <f t="shared" ref="O3:O17" si="2">IFERROR(IF($K3=1,0,IF(($C$1-$K3)/($M3-$K3)&lt;-0.005,100%,IF(($C$1-$K3)/($M3-$K3)&gt;100%,100%,($C$1-$K3)/($L3-$K3)))),0)</f>
-        <v>0.6481715006</v>
+        <v>0.6500630517</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
@@ -970,7 +999,7 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" si="2"/>
-        <v>0.6648275862</v>
+        <v>0.6689655172</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
@@ -1015,7 +1044,7 @@
       </c>
       <c r="O6" s="13">
         <f t="shared" si="2"/>
-        <v>0.4817021277</v>
+        <v>0.4842553191</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
@@ -1060,7 +1089,7 @@
       </c>
       <c r="O7" s="13">
         <f t="shared" si="2"/>
-        <v>0.9110287303</v>
+        <v>0.9138090825</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
@@ -1150,7 +1179,7 @@
       </c>
       <c r="O9" s="13">
         <f t="shared" si="2"/>
-        <v>0.8552412646</v>
+        <v>0.8577371048</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
@@ -1240,7 +1269,7 @@
       </c>
       <c r="O11" s="13">
         <f t="shared" si="2"/>
-        <v>0.9930875576</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="1">
@@ -1285,7 +1314,7 @@
       </c>
       <c r="O12" s="13">
         <f t="shared" si="2"/>
-        <v>0.2955465587</v>
+        <v>0.3016194332</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="1">
@@ -1330,7 +1359,7 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" si="2"/>
-        <v>0.4098360656</v>
+        <v>0.4196721311</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="1">
@@ -1375,7 +1404,7 @@
       </c>
       <c r="O14" s="13">
         <f t="shared" si="2"/>
-        <v>0.9981197117</v>
+        <v>0.9990598558</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
@@ -1420,7 +1449,7 @@
       </c>
       <c r="O15" s="13">
         <f t="shared" si="2"/>
-        <v>0.7775905644</v>
+        <v>0.7801179444</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -1465,7 +1494,7 @@
       </c>
       <c r="O16" s="13">
         <f t="shared" si="2"/>
-        <v>0.7775905644</v>
+        <v>0.7801179444</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1510,7 +1539,7 @@
       </c>
       <c r="O17" s="13">
         <f t="shared" si="2"/>
-        <v>0.7775905644</v>
+        <v>0.7801179444</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
@@ -1634,135 +1663,319 @@
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19" t="s">
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="19" t="s">
+      <c r="H23" s="16"/>
+      <c r="I23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="23">
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="17">
         <v>0.77</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="6"/>
+      <c r="C24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19" t="s">
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="19" t="s">
+      <c r="H24" s="16"/>
+      <c r="I24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="23">
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="17">
         <v>0.77</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="B25" s="24"/>
-      <c r="C25" s="25" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="25" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H25" s="24"/>
-      <c r="I25" s="26" t="s">
+      <c r="H25" s="18"/>
+      <c r="I25" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="28">
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="21">
         <v>0.77</v>
       </c>
-      <c r="P25" s="29"/>
+      <c r="P25" s="22"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="B26" s="24"/>
-      <c r="C26" s="25" t="s">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="26" t="s">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="26" t="s">
+      <c r="H26" s="18"/>
+      <c r="I26" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="28">
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="21">
         <v>0.77</v>
       </c>
-      <c r="P26" s="29"/>
+      <c r="P26" s="22"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="B27" s="24"/>
-      <c r="C27" s="25" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="24"/>
-      <c r="I27" s="26" t="s">
+      <c r="H27" s="18"/>
+      <c r="I27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="28">
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="21">
         <v>0.77</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="B28" s="23"/>
+      <c r="C28" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="I28" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="B29" s="23"/>
+      <c r="C29" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="23"/>
+      <c r="I29" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="B30" s="23"/>
+      <c r="C30" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="B31" s="23"/>
+      <c r="C31" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="23"/>
+      <c r="I31" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="B32" s="23"/>
+      <c r="C32" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="23"/>
+      <c r="I32" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="B33" s="23"/>
+      <c r="C33" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="23"/>
+      <c r="I33" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="B34" s="23"/>
+      <c r="C34" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="23"/>
+      <c r="I34" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="B35" s="23"/>
+      <c r="C35" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" s="23"/>
+      <c r="I35" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="26">
+        <v>0.0</v>
+      </c>
+    </row>
     <row r="36" ht="14.25" customHeight="1"/>
     <row r="37" ht="14.25" customHeight="1"/>
     <row r="38" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
change back to 2 capitalizations for each, so blank healths are counted as green
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
   <si>
     <t>Today's date:</t>
   </si>
@@ -260,55 +260,10 @@
     <t>o2</t>
   </si>
   <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>a5</t>
-  </si>
-  <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>InfoSec Protection Services</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>IT Risk Management</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>q4</t>
-  </si>
-  <si>
-    <t>q5</t>
-  </si>
-  <si>
-    <t>q6</t>
-  </si>
-  <si>
-    <t>q7</t>
-  </si>
-  <si>
-    <t>Security Design Services</t>
-  </si>
-  <si>
-    <t>q8</t>
-  </si>
-  <si>
-    <t>Compliance &amp; Assurance</t>
+    <t>o3</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -344,7 +299,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,12 +324,6 @@
         <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC1E4F5"/>
-        <bgColor rgb="FFC1E4F5"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -388,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -429,28 +378,22 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,7 +499,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O35" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B2:O24" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="14">
     <tableColumn name="Project _x000a_ID" id="1"/>
     <tableColumn name="Project Name" id="2"/>
@@ -808,7 +751,7 @@
       </c>
       <c r="C1" s="2">
         <f>TODAY()</f>
-        <v>45503</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="2" ht="58.5" customHeight="1">
@@ -909,7 +852,7 @@
       </c>
       <c r="O3" s="13">
         <f t="shared" ref="O3:O17" si="2">IFERROR(IF($K3=1,0,IF(($C$1-$K3)/($M3-$K3)&lt;-0.005,100%,IF(($C$1-$K3)/($M3-$K3)&gt;100%,100%,($C$1-$K3)/($L3-$K3)))),0)</f>
-        <v>0.6500630517</v>
+        <v>0.657629256</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
@@ -999,7 +942,7 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" si="2"/>
-        <v>0.6689655172</v>
+        <v>0.6855172414</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
@@ -1044,7 +987,7 @@
       </c>
       <c r="O6" s="13">
         <f t="shared" si="2"/>
-        <v>0.4842553191</v>
+        <v>0.4944680851</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
@@ -1089,7 +1032,7 @@
       </c>
       <c r="O7" s="13">
         <f t="shared" si="2"/>
-        <v>0.9138090825</v>
+        <v>0.9249304912</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
@@ -1179,7 +1122,7 @@
       </c>
       <c r="O9" s="13">
         <f t="shared" si="2"/>
-        <v>0.8577371048</v>
+        <v>0.8677204659</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
@@ -1314,7 +1257,7 @@
       </c>
       <c r="O12" s="13">
         <f t="shared" si="2"/>
-        <v>0.3016194332</v>
+        <v>0.3259109312</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="1">
@@ -1359,7 +1302,7 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" si="2"/>
-        <v>0.4196721311</v>
+        <v>0.4590163934</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="1">
@@ -1404,7 +1347,7 @@
       </c>
       <c r="O14" s="13">
         <f t="shared" si="2"/>
-        <v>0.9990598558</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
@@ -1449,7 +1392,7 @@
       </c>
       <c r="O15" s="13">
         <f t="shared" si="2"/>
-        <v>0.7801179444</v>
+        <v>0.7902274642</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -1494,7 +1437,7 @@
       </c>
       <c r="O16" s="13">
         <f t="shared" si="2"/>
-        <v>0.7801179444</v>
+        <v>0.7902274642</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1539,7 +1482,7 @@
       </c>
       <c r="O17" s="13">
         <f t="shared" si="2"/>
-        <v>0.7801179444</v>
+        <v>0.7902274642</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
@@ -1663,319 +1606,62 @@
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="B23" s="6"/>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="8" t="s">
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="20"/>
+      <c r="I23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="17">
-        <v>0.77</v>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="23">
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="B24" s="6"/>
-      <c r="C24" s="8" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="17">
-        <v>0.77</v>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="23">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" s="18"/>
-      <c r="I25" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="21">
-        <v>0.77</v>
-      </c>
-      <c r="P25" s="22"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="21">
-        <v>0.77</v>
-      </c>
-      <c r="P26" s="22"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="21">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="B28" s="23"/>
-      <c r="C28" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="B29" s="23"/>
-      <c r="C29" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="B30" s="23"/>
-      <c r="C30" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="B31" s="23"/>
-      <c r="C31" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="B32" s="23"/>
-      <c r="C32" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="B33" s="23"/>
-      <c r="C33" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H33" s="23"/>
-      <c r="I33" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="B34" s="23"/>
-      <c r="C34" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" s="23"/>
-      <c r="I34" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="B35" s="23"/>
-      <c r="C35" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" s="23"/>
-      <c r="I35" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="26">
-        <v>0.0</v>
-      </c>
-    </row>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
     <row r="36" ht="14.25" customHeight="1"/>
     <row r="37" ht="14.25" customHeight="1"/>
     <row r="38" ht="14.25" customHeight="1"/>

</xml_diff>